<commit_message>
Sparkles: Features: Add Auth credentials, users and obs functions
</commit_message>
<xml_diff>
--- a/static/templates/PLANTILLA - INCIDENCIAS.xlsx
+++ b/static/templates/PLANTILLA - INCIDENCIAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documentos\work_projects\medileser\aplicativoSmart\backSmart\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2231794-B823-4EE8-8A2D-C18344C3E253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620C2948-BB43-4011-9F15-A356FC260B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E90C098F-6B10-452D-A8F9-584E2FD75B0A}"/>
+    <workbookView xWindow="345" yWindow="4320" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{E90C098F-6B10-452D-A8F9-584E2FD75B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="CALLAO AGOSTO" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>TIEMPO DE INCIDENCIA</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>APERTURA DE TAPA</t>
+  </si>
+  <si>
+    <t>MEDIDOR SIN CONEXION</t>
   </si>
 </sst>
 </file>
@@ -856,7 +859,7 @@
   </sheetPr>
   <dimension ref="A1:K2889"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -30266,13 +30269,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687A9B8B-C5BD-477B-817E-371AAA3056E6}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -30375,6 +30380,11 @@
         <v>28</v>
       </c>
     </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>